<commit_message>
last-minute updates from Wed
</commit_message>
<xml_diff>
--- a/Lab7/Lab7BoM v2.xlsx
+++ b/Lab7/Lab7BoM v2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39EE19C-E140-403C-8991-CF2712494CA3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E83369-2263-4511-B512-A507431B9266}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="141">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -256,24 +256,6 @@
     <t>MakerSpace</t>
   </si>
   <si>
-    <t>ACCELER DUAL-AX 2.0G 8PLCC</t>
-  </si>
-  <si>
-    <t>Analog Devices</t>
-  </si>
-  <si>
-    <t>ADXL202JQC</t>
-  </si>
-  <si>
-    <t>Quest Components</t>
-  </si>
-  <si>
-    <t>ADXL202</t>
-  </si>
-  <si>
-    <t>Valvano</t>
-  </si>
-  <si>
     <t>L293 Motor H bridge</t>
   </si>
   <si>
@@ -421,12 +403,6 @@
     <t>http://users.ece.utexas.edu/~valvano/Datasheets/L293d.pdf</t>
   </si>
   <si>
-    <t>http://www.analog.com/media/en/technical-documentation/obsolete-data-sheets/ADXL210.pdf (obsolete?)</t>
-  </si>
-  <si>
-    <t>0.6 mA</t>
-  </si>
-  <si>
     <t>200 mA ?</t>
   </si>
   <si>
@@ -461,6 +437,12 @@
   </si>
   <si>
     <t>IN053</t>
+  </si>
+  <si>
+    <t>Motor Battery Connection</t>
+  </si>
+  <si>
+    <t>PowerHeader</t>
   </si>
 </sst>
 </file>
@@ -849,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,10 +902,10 @@
         <v>13</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -934,13 +916,13 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I4" s="7">
         <v>2.5</v>
@@ -952,10 +934,10 @@
         <v>76</v>
       </c>
       <c r="N4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="O4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -963,16 +945,16 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I5" s="7">
         <v>8.76</v>
@@ -984,10 +966,10 @@
         <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1020,10 +1002,10 @@
         <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="O6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1082,10 +1064,10 @@
         <v>39</v>
       </c>
       <c r="N8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="O8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1096,19 +1078,19 @@
         <v>69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I9" s="5">
         <v>3.5</v>
@@ -1118,16 +1100,16 @@
         <v>3.5</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="N9" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="O9" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1135,16 +1117,16 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E10" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I10" s="7">
         <v>2.81</v>
@@ -1161,13 +1143,13 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I11" s="7">
         <v>0.5</v>
@@ -1248,10 +1230,10 @@
         <v>31</v>
       </c>
       <c r="N13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="O13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1259,13 +1241,13 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I14" s="7">
         <v>4.99</v>
@@ -1285,7 +1267,7 @@
         <v>65</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>60</v>
@@ -1313,10 +1295,10 @@
         <v>31</v>
       </c>
       <c r="N15" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="O15" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1361,19 +1343,19 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I17" s="5">
         <v>0.11</v>
@@ -1392,19 +1374,19 @@
         <v>2</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I18" s="5">
         <v>0.26</v>
@@ -1414,7 +1396,7 @@
         <v>0.52</v>
       </c>
       <c r="K18" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1453,10 +1435,10 @@
         <v>31</v>
       </c>
       <c r="N19" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="O19" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1495,10 +1477,10 @@
         <v>31</v>
       </c>
       <c r="N20" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="O20" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1537,10 +1519,10 @@
         <v>31</v>
       </c>
       <c r="N21" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O21" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1551,7 +1533,7 @@
         <v>67</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1575,10 +1557,10 @@
         <v>31</v>
       </c>
       <c r="N22" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="O22" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1617,75 +1599,52 @@
         <v>31</v>
       </c>
       <c r="N23" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="O23" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I24" s="5">
-        <v>7.5</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" si="6"/>
-        <v>7.5</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
       <c r="K24" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="N24" t="s">
-        <v>134</v>
-      </c>
-      <c r="O24" t="s">
-        <v>133</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I25" s="5">
         <v>0.05</v>
@@ -1695,16 +1654,16 @@
         <v>0.1</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="N25" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="O25" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>